<commit_message>
update macros countries, system tab
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\add-in-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03212FDA-B06F-4C29-BD6D-0883BBFC5288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E399FB5-0D9D-4E77-BBA7-E29B7E424236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
add macros to TabMain
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr codeName="ЭтаКнига"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\add-in-dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\dev.xlam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E399FB5-0D9D-4E77-BBA7-E29B7E424236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E2C96B-7792-484E-AB66-9571B9E8841A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PL" sheetId="4" r:id="rId1"/>
+    <sheet name="1" sheetId="4" r:id="rId1"/>
     <sheet name="PL Сокр (1)" sheetId="9" r:id="rId2"/>
     <sheet name="Лист1" sheetId="5" r:id="rId3"/>
   </sheets>
@@ -1367,7 +1367,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1389,6 +1389,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1422,7 +1428,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1480,10 +1486,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 5" xfId="1" xr:uid="{6209055A-769B-44BD-B3E1-1FC7025223BD}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2 3" xfId="2" xr:uid="{6FFC2D92-5A8F-448E-BF28-3B2AE5FAB196}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1767,7 +1776,7 @@
   </sheetPr>
   <dimension ref="A1:O992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -8992,7 +9001,7 @@
   </sheetPr>
   <dimension ref="A1:O992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -9370,7 +9379,7 @@
         <v>229</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>

</xml_diff>

<commit_message>
implent new correct dursun markas db into dict
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\my-AddIn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1BD136-2BC6-4C87-BC68-1DFFF330A3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57224509-67CB-4B1C-82E9-C9DB728E7FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="749" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5974,10 +5974,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10334,7 +10334,7 @@
   <dimension ref="A1:O778"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -27798,14 +27798,14 @@
       <c r="E7" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="80" t="s">
+      <c r="F7" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80" t="s">
+      <c r="G7" s="79"/>
+      <c r="H7" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="80"/>
+      <c r="I7" s="79"/>
       <c r="J7" s="48" t="s">
         <v>6</v>
       </c>
@@ -32924,10 +32924,10 @@
       <c r="G128" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H128" s="79">
+      <c r="H128" s="80">
         <v>20</v>
       </c>
-      <c r="I128" s="79" t="s">
+      <c r="I128" s="80" t="s">
         <v>806</v>
       </c>
       <c r="J128" s="57">
@@ -33095,8 +33095,8 @@
       <c r="G129" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H129" s="79"/>
-      <c r="I129" s="79"/>
+      <c r="H129" s="80"/>
+      <c r="I129" s="80"/>
       <c r="J129" s="57">
         <v>13</v>
       </c>
@@ -33262,8 +33262,8 @@
       <c r="G130" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H130" s="79"/>
-      <c r="I130" s="79"/>
+      <c r="H130" s="80"/>
+      <c r="I130" s="80"/>
       <c r="J130" s="57">
         <v>0.66</v>
       </c>
@@ -33429,8 +33429,8 @@
       <c r="G131" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H131" s="79"/>
-      <c r="I131" s="79"/>
+      <c r="H131" s="80"/>
+      <c r="I131" s="80"/>
       <c r="J131" s="57">
         <v>0.52</v>
       </c>
@@ -33596,8 +33596,8 @@
       <c r="G132" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H132" s="79"/>
-      <c r="I132" s="79"/>
+      <c r="H132" s="80"/>
+      <c r="I132" s="80"/>
       <c r="J132" s="57">
         <v>53</v>
       </c>
@@ -33763,8 +33763,8 @@
       <c r="G133" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H133" s="79"/>
-      <c r="I133" s="79"/>
+      <c r="H133" s="80"/>
+      <c r="I133" s="80"/>
       <c r="J133" s="57">
         <v>3.5</v>
       </c>
@@ -33930,8 +33930,8 @@
       <c r="G134" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H134" s="79"/>
-      <c r="I134" s="79"/>
+      <c r="H134" s="80"/>
+      <c r="I134" s="80"/>
       <c r="J134" s="57">
         <v>0.31</v>
       </c>
@@ -34097,8 +34097,8 @@
       <c r="G135" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H135" s="79"/>
-      <c r="I135" s="79"/>
+      <c r="H135" s="80"/>
+      <c r="I135" s="80"/>
       <c r="J135" s="57">
         <v>4</v>
       </c>
@@ -34264,8 +34264,8 @@
       <c r="G136" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H136" s="79"/>
-      <c r="I136" s="79"/>
+      <c r="H136" s="80"/>
+      <c r="I136" s="80"/>
       <c r="J136" s="57">
         <v>0.4</v>
       </c>
@@ -34431,8 +34431,8 @@
       <c r="G137" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H137" s="79"/>
-      <c r="I137" s="79"/>
+      <c r="H137" s="80"/>
+      <c r="I137" s="80"/>
       <c r="J137" s="57">
         <v>1.17</v>
       </c>
@@ -34598,8 +34598,8 @@
       <c r="G138" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H138" s="79"/>
-      <c r="I138" s="79"/>
+      <c r="H138" s="80"/>
+      <c r="I138" s="80"/>
       <c r="J138" s="57">
         <v>0.14000000000000001</v>
       </c>
@@ -34765,8 +34765,8 @@
       <c r="G139" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H139" s="79"/>
-      <c r="I139" s="79"/>
+      <c r="H139" s="80"/>
+      <c r="I139" s="80"/>
       <c r="J139" s="57">
         <v>0.06</v>
       </c>
@@ -34932,8 +34932,8 @@
       <c r="G140" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H140" s="79"/>
-      <c r="I140" s="79"/>
+      <c r="H140" s="80"/>
+      <c r="I140" s="80"/>
       <c r="J140" s="57">
         <v>0.18</v>
       </c>
@@ -35099,8 +35099,8 @@
       <c r="G141" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H141" s="79"/>
-      <c r="I141" s="79"/>
+      <c r="H141" s="80"/>
+      <c r="I141" s="80"/>
       <c r="J141" s="57">
         <v>0.04</v>
       </c>
@@ -35266,8 +35266,8 @@
       <c r="G142" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H142" s="79"/>
-      <c r="I142" s="79"/>
+      <c r="H142" s="80"/>
+      <c r="I142" s="80"/>
       <c r="J142" s="57">
         <v>25</v>
       </c>
@@ -35433,8 +35433,8 @@
       <c r="G143" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H143" s="79"/>
-      <c r="I143" s="79"/>
+      <c r="H143" s="80"/>
+      <c r="I143" s="80"/>
       <c r="J143" s="57">
         <v>0.18</v>
       </c>
@@ -35600,8 +35600,8 @@
       <c r="G144" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H144" s="79"/>
-      <c r="I144" s="79"/>
+      <c r="H144" s="80"/>
+      <c r="I144" s="80"/>
       <c r="J144" s="57">
         <v>0.21</v>
       </c>
@@ -35767,8 +35767,8 @@
       <c r="G145" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H145" s="79"/>
-      <c r="I145" s="79"/>
+      <c r="H145" s="80"/>
+      <c r="I145" s="80"/>
       <c r="J145" s="57">
         <v>0.15</v>
       </c>
@@ -35934,8 +35934,8 @@
       <c r="G146" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H146" s="79"/>
-      <c r="I146" s="79"/>
+      <c r="H146" s="80"/>
+      <c r="I146" s="80"/>
       <c r="J146" s="57">
         <v>0.34</v>
       </c>
@@ -36101,8 +36101,8 @@
       <c r="G147" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H147" s="79"/>
-      <c r="I147" s="79"/>
+      <c r="H147" s="80"/>
+      <c r="I147" s="80"/>
       <c r="J147" s="57">
         <v>0.06</v>
       </c>
@@ -36268,8 +36268,8 @@
       <c r="G148" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H148" s="79"/>
-      <c r="I148" s="79"/>
+      <c r="H148" s="80"/>
+      <c r="I148" s="80"/>
       <c r="J148" s="57">
         <v>0.11</v>
       </c>
@@ -36435,8 +36435,8 @@
       <c r="G149" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H149" s="79"/>
-      <c r="I149" s="79"/>
+      <c r="H149" s="80"/>
+      <c r="I149" s="80"/>
       <c r="J149" s="57">
         <v>0.18</v>
       </c>
@@ -36602,8 +36602,8 @@
       <c r="G150" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H150" s="79"/>
-      <c r="I150" s="79"/>
+      <c r="H150" s="80"/>
+      <c r="I150" s="80"/>
       <c r="J150" s="57">
         <v>0.16</v>
       </c>
@@ -36769,8 +36769,8 @@
       <c r="G151" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H151" s="79"/>
-      <c r="I151" s="79"/>
+      <c r="H151" s="80"/>
+      <c r="I151" s="80"/>
       <c r="J151" s="57">
         <v>3</v>
       </c>
@@ -36936,8 +36936,8 @@
       <c r="G152" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H152" s="79"/>
-      <c r="I152" s="79"/>
+      <c r="H152" s="80"/>
+      <c r="I152" s="80"/>
       <c r="J152" s="57">
         <v>0.08</v>
       </c>
@@ -37103,8 +37103,8 @@
       <c r="G153" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H153" s="79"/>
-      <c r="I153" s="79"/>
+      <c r="H153" s="80"/>
+      <c r="I153" s="80"/>
       <c r="J153" s="57">
         <v>0.4</v>
       </c>
@@ -37270,8 +37270,8 @@
       <c r="G154" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H154" s="79"/>
-      <c r="I154" s="79"/>
+      <c r="H154" s="80"/>
+      <c r="I154" s="80"/>
       <c r="J154" s="57">
         <v>1.6</v>
       </c>
@@ -37437,8 +37437,8 @@
       <c r="G155" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H155" s="79"/>
-      <c r="I155" s="79"/>
+      <c r="H155" s="80"/>
+      <c r="I155" s="80"/>
       <c r="J155" s="57">
         <v>2.1</v>
       </c>
@@ -37604,8 +37604,8 @@
       <c r="G156" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H156" s="79"/>
-      <c r="I156" s="79"/>
+      <c r="H156" s="80"/>
+      <c r="I156" s="80"/>
       <c r="J156" s="57">
         <v>0.2</v>
       </c>
@@ -37771,8 +37771,8 @@
       <c r="G157" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H157" s="79"/>
-      <c r="I157" s="79"/>
+      <c r="H157" s="80"/>
+      <c r="I157" s="80"/>
       <c r="J157" s="57">
         <v>3</v>
       </c>
@@ -37938,8 +37938,8 @@
       <c r="G158" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H158" s="79"/>
-      <c r="I158" s="79"/>
+      <c r="H158" s="80"/>
+      <c r="I158" s="80"/>
       <c r="J158" s="57">
         <v>7</v>
       </c>
@@ -38105,8 +38105,8 @@
       <c r="G159" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H159" s="79"/>
-      <c r="I159" s="79"/>
+      <c r="H159" s="80"/>
+      <c r="I159" s="80"/>
       <c r="J159" s="57">
         <v>2.5</v>
       </c>
@@ -38272,8 +38272,8 @@
       <c r="G160" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H160" s="79"/>
-      <c r="I160" s="79"/>
+      <c r="H160" s="80"/>
+      <c r="I160" s="80"/>
       <c r="J160" s="57">
         <v>0.8</v>
       </c>
@@ -38439,8 +38439,8 @@
       <c r="G161" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H161" s="79"/>
-      <c r="I161" s="79"/>
+      <c r="H161" s="80"/>
+      <c r="I161" s="80"/>
       <c r="J161" s="57">
         <v>0.32</v>
       </c>
@@ -38606,8 +38606,8 @@
       <c r="G162" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H162" s="79"/>
-      <c r="I162" s="79"/>
+      <c r="H162" s="80"/>
+      <c r="I162" s="80"/>
       <c r="J162" s="57">
         <v>0.05</v>
       </c>
@@ -38773,8 +38773,8 @@
       <c r="G163" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H163" s="79"/>
-      <c r="I163" s="79"/>
+      <c r="H163" s="80"/>
+      <c r="I163" s="80"/>
       <c r="J163" s="57">
         <v>0.9</v>
       </c>
@@ -38940,8 +38940,8 @@
       <c r="G164" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H164" s="79"/>
-      <c r="I164" s="79"/>
+      <c r="H164" s="80"/>
+      <c r="I164" s="80"/>
       <c r="J164" s="57">
         <v>3.5</v>
       </c>
@@ -39107,8 +39107,8 @@
       <c r="G165" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H165" s="79"/>
-      <c r="I165" s="79"/>
+      <c r="H165" s="80"/>
+      <c r="I165" s="80"/>
       <c r="J165" s="57">
         <v>0.04</v>
       </c>
@@ -39274,8 +39274,8 @@
       <c r="G166" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H166" s="79"/>
-      <c r="I166" s="79"/>
+      <c r="H166" s="80"/>
+      <c r="I166" s="80"/>
       <c r="J166" s="57">
         <v>0.04</v>
       </c>
@@ -39441,8 +39441,8 @@
       <c r="G167" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H167" s="79"/>
-      <c r="I167" s="79"/>
+      <c r="H167" s="80"/>
+      <c r="I167" s="80"/>
       <c r="J167" s="57">
         <v>1.08</v>
       </c>
@@ -39608,8 +39608,8 @@
       <c r="G168" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H168" s="79"/>
-      <c r="I168" s="79"/>
+      <c r="H168" s="80"/>
+      <c r="I168" s="80"/>
       <c r="J168" s="57">
         <v>2</v>
       </c>
@@ -39775,8 +39775,8 @@
       <c r="G169" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H169" s="79"/>
-      <c r="I169" s="79"/>
+      <c r="H169" s="80"/>
+      <c r="I169" s="80"/>
       <c r="J169" s="57">
         <v>14</v>
       </c>
@@ -39942,8 +39942,8 @@
       <c r="G170" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H170" s="79"/>
-      <c r="I170" s="79"/>
+      <c r="H170" s="80"/>
+      <c r="I170" s="80"/>
       <c r="J170" s="57">
         <v>0.28000000000000003</v>
       </c>
@@ -40109,8 +40109,8 @@
       <c r="G171" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H171" s="79"/>
-      <c r="I171" s="79"/>
+      <c r="H171" s="80"/>
+      <c r="I171" s="80"/>
       <c r="J171" s="57">
         <v>0.02</v>
       </c>
@@ -40276,8 +40276,8 @@
       <c r="G172" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H172" s="79"/>
-      <c r="I172" s="79"/>
+      <c r="H172" s="80"/>
+      <c r="I172" s="80"/>
       <c r="J172" s="57">
         <v>0.02</v>
       </c>
@@ -40443,8 +40443,8 @@
       <c r="G173" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H173" s="79"/>
-      <c r="I173" s="79"/>
+      <c r="H173" s="80"/>
+      <c r="I173" s="80"/>
       <c r="J173" s="57">
         <v>0.05</v>
       </c>
@@ -40610,8 +40610,8 @@
       <c r="G174" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H174" s="79"/>
-      <c r="I174" s="79"/>
+      <c r="H174" s="80"/>
+      <c r="I174" s="80"/>
       <c r="J174" s="57">
         <v>0.3</v>
       </c>
@@ -40777,8 +40777,8 @@
       <c r="G175" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H175" s="79"/>
-      <c r="I175" s="79"/>
+      <c r="H175" s="80"/>
+      <c r="I175" s="80"/>
       <c r="J175" s="57">
         <v>0.04</v>
       </c>
@@ -40944,8 +40944,8 @@
       <c r="G176" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H176" s="79"/>
-      <c r="I176" s="79"/>
+      <c r="H176" s="80"/>
+      <c r="I176" s="80"/>
       <c r="J176" s="57">
         <v>0.05</v>
       </c>
@@ -41111,8 +41111,8 @@
       <c r="G177" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H177" s="79"/>
-      <c r="I177" s="79"/>
+      <c r="H177" s="80"/>
+      <c r="I177" s="80"/>
       <c r="J177" s="57">
         <v>0.09</v>
       </c>
@@ -41278,8 +41278,8 @@
       <c r="G178" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H178" s="79"/>
-      <c r="I178" s="79"/>
+      <c r="H178" s="80"/>
+      <c r="I178" s="80"/>
       <c r="J178" s="57">
         <v>0.26</v>
       </c>
@@ -41445,8 +41445,8 @@
       <c r="G179" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H179" s="79"/>
-      <c r="I179" s="79"/>
+      <c r="H179" s="80"/>
+      <c r="I179" s="80"/>
       <c r="J179" s="57">
         <v>2.1</v>
       </c>
@@ -41612,8 +41612,8 @@
       <c r="G180" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H180" s="79"/>
-      <c r="I180" s="79"/>
+      <c r="H180" s="80"/>
+      <c r="I180" s="80"/>
       <c r="J180" s="57">
         <v>0.23</v>
       </c>
@@ -41779,8 +41779,8 @@
       <c r="G181" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H181" s="79"/>
-      <c r="I181" s="79"/>
+      <c r="H181" s="80"/>
+      <c r="I181" s="80"/>
       <c r="J181" s="57">
         <v>0.17</v>
       </c>
@@ -41946,8 +41946,8 @@
       <c r="G182" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H182" s="79"/>
-      <c r="I182" s="79"/>
+      <c r="H182" s="80"/>
+      <c r="I182" s="80"/>
       <c r="J182" s="57">
         <v>0.24</v>
       </c>
@@ -42113,8 +42113,8 @@
       <c r="G183" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H183" s="79"/>
-      <c r="I183" s="79"/>
+      <c r="H183" s="80"/>
+      <c r="I183" s="80"/>
       <c r="J183" s="57">
         <v>0.24</v>
       </c>
@@ -42280,8 +42280,8 @@
       <c r="G184" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H184" s="79"/>
-      <c r="I184" s="79"/>
+      <c r="H184" s="80"/>
+      <c r="I184" s="80"/>
       <c r="J184" s="57">
         <v>0.48</v>
       </c>
@@ -42447,8 +42447,8 @@
       <c r="G185" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H185" s="79"/>
-      <c r="I185" s="79"/>
+      <c r="H185" s="80"/>
+      <c r="I185" s="80"/>
       <c r="J185" s="57">
         <v>0.27</v>
       </c>
@@ -42614,8 +42614,8 @@
       <c r="G186" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H186" s="79"/>
-      <c r="I186" s="79"/>
+      <c r="H186" s="80"/>
+      <c r="I186" s="80"/>
       <c r="J186" s="57">
         <v>0.68</v>
       </c>
@@ -42781,8 +42781,8 @@
       <c r="G187" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H187" s="79"/>
-      <c r="I187" s="79"/>
+      <c r="H187" s="80"/>
+      <c r="I187" s="80"/>
       <c r="J187" s="57">
         <v>2.5</v>
       </c>
@@ -42948,8 +42948,8 @@
       <c r="G188" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H188" s="79"/>
-      <c r="I188" s="79"/>
+      <c r="H188" s="80"/>
+      <c r="I188" s="80"/>
       <c r="J188" s="57">
         <v>0.18</v>
       </c>
@@ -43115,8 +43115,8 @@
       <c r="G189" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H189" s="79"/>
-      <c r="I189" s="79"/>
+      <c r="H189" s="80"/>
+      <c r="I189" s="80"/>
       <c r="J189" s="57">
         <v>0.08</v>
       </c>
@@ -43282,8 +43282,8 @@
       <c r="G190" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H190" s="79"/>
-      <c r="I190" s="79"/>
+      <c r="H190" s="80"/>
+      <c r="I190" s="80"/>
       <c r="J190" s="57">
         <v>0.3</v>
       </c>
@@ -43449,8 +43449,8 @@
       <c r="G191" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H191" s="79"/>
-      <c r="I191" s="79"/>
+      <c r="H191" s="80"/>
+      <c r="I191" s="80"/>
       <c r="J191" s="57">
         <v>0.75</v>
       </c>
@@ -43616,8 +43616,8 @@
       <c r="G192" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H192" s="79"/>
-      <c r="I192" s="79"/>
+      <c r="H192" s="80"/>
+      <c r="I192" s="80"/>
       <c r="J192" s="57">
         <v>0.1</v>
       </c>
@@ -43783,8 +43783,8 @@
       <c r="G193" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H193" s="79"/>
-      <c r="I193" s="79"/>
+      <c r="H193" s="80"/>
+      <c r="I193" s="80"/>
       <c r="J193" s="57">
         <v>0.06</v>
       </c>
@@ -43950,8 +43950,8 @@
       <c r="G194" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H194" s="79"/>
-      <c r="I194" s="79"/>
+      <c r="H194" s="80"/>
+      <c r="I194" s="80"/>
       <c r="J194" s="57">
         <v>0.1</v>
       </c>
@@ -44117,8 +44117,8 @@
       <c r="G195" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H195" s="79"/>
-      <c r="I195" s="79"/>
+      <c r="H195" s="80"/>
+      <c r="I195" s="80"/>
       <c r="J195" s="57">
         <v>0.28000000000000003</v>
       </c>
@@ -44284,8 +44284,8 @@
       <c r="G196" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H196" s="79"/>
-      <c r="I196" s="79"/>
+      <c r="H196" s="80"/>
+      <c r="I196" s="80"/>
       <c r="J196" s="57">
         <v>0.34</v>
       </c>
@@ -44451,8 +44451,8 @@
       <c r="G197" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H197" s="79"/>
-      <c r="I197" s="79"/>
+      <c r="H197" s="80"/>
+      <c r="I197" s="80"/>
       <c r="J197" s="57">
         <v>0.48</v>
       </c>
@@ -44618,8 +44618,8 @@
       <c r="G198" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H198" s="79"/>
-      <c r="I198" s="79"/>
+      <c r="H198" s="80"/>
+      <c r="I198" s="80"/>
       <c r="J198" s="57">
         <v>0.21</v>
       </c>
@@ -44785,8 +44785,8 @@
       <c r="G199" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H199" s="79"/>
-      <c r="I199" s="79"/>
+      <c r="H199" s="80"/>
+      <c r="I199" s="80"/>
       <c r="J199" s="57">
         <v>0.06</v>
       </c>
@@ -44952,8 +44952,8 @@
       <c r="G200" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H200" s="79"/>
-      <c r="I200" s="79"/>
+      <c r="H200" s="80"/>
+      <c r="I200" s="80"/>
       <c r="J200" s="57">
         <v>0.4</v>
       </c>
@@ -45119,8 +45119,8 @@
       <c r="G201" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H201" s="79"/>
-      <c r="I201" s="79"/>
+      <c r="H201" s="80"/>
+      <c r="I201" s="80"/>
       <c r="J201" s="57">
         <v>0.06</v>
       </c>
@@ -45286,8 +45286,8 @@
       <c r="G202" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H202" s="79"/>
-      <c r="I202" s="79"/>
+      <c r="H202" s="80"/>
+      <c r="I202" s="80"/>
       <c r="J202" s="57">
         <v>23</v>
       </c>
@@ -45453,8 +45453,8 @@
       <c r="G203" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H203" s="79"/>
-      <c r="I203" s="79"/>
+      <c r="H203" s="80"/>
+      <c r="I203" s="80"/>
       <c r="J203" s="57">
         <v>1.4</v>
       </c>
@@ -45620,8 +45620,8 @@
       <c r="G204" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H204" s="79"/>
-      <c r="I204" s="79"/>
+      <c r="H204" s="80"/>
+      <c r="I204" s="80"/>
       <c r="J204" s="57">
         <v>0.02</v>
       </c>
@@ -45787,8 +45787,8 @@
       <c r="G205" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H205" s="79"/>
-      <c r="I205" s="79"/>
+      <c r="H205" s="80"/>
+      <c r="I205" s="80"/>
       <c r="J205" s="57">
         <v>5.32</v>
       </c>
@@ -45954,8 +45954,8 @@
       <c r="G206" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H206" s="79"/>
-      <c r="I206" s="79"/>
+      <c r="H206" s="80"/>
+      <c r="I206" s="80"/>
       <c r="J206" s="57">
         <v>0.9</v>
       </c>
@@ -46121,8 +46121,8 @@
       <c r="G207" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H207" s="79"/>
-      <c r="I207" s="79"/>
+      <c r="H207" s="80"/>
+      <c r="I207" s="80"/>
       <c r="J207" s="57">
         <v>2.25</v>
       </c>
@@ -46288,8 +46288,8 @@
       <c r="G208" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H208" s="79"/>
-      <c r="I208" s="79"/>
+      <c r="H208" s="80"/>
+      <c r="I208" s="80"/>
       <c r="J208" s="57">
         <v>0.2</v>
       </c>
@@ -46455,8 +46455,8 @@
       <c r="G209" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H209" s="79"/>
-      <c r="I209" s="79"/>
+      <c r="H209" s="80"/>
+      <c r="I209" s="80"/>
       <c r="J209" s="57">
         <v>0.12</v>
       </c>
@@ -46622,8 +46622,8 @@
       <c r="G210" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H210" s="79"/>
-      <c r="I210" s="79"/>
+      <c r="H210" s="80"/>
+      <c r="I210" s="80"/>
       <c r="J210" s="57">
         <v>0.25</v>
       </c>
@@ -46789,8 +46789,8 @@
       <c r="G211" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H211" s="79"/>
-      <c r="I211" s="79"/>
+      <c r="H211" s="80"/>
+      <c r="I211" s="80"/>
       <c r="J211" s="57">
         <v>0.01</v>
       </c>
@@ -46956,8 +46956,8 @@
       <c r="G212" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H212" s="79"/>
-      <c r="I212" s="79"/>
+      <c r="H212" s="80"/>
+      <c r="I212" s="80"/>
       <c r="J212" s="57">
         <v>0.32</v>
       </c>
@@ -47123,8 +47123,8 @@
       <c r="G213" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H213" s="79"/>
-      <c r="I213" s="79"/>
+      <c r="H213" s="80"/>
+      <c r="I213" s="80"/>
       <c r="J213" s="57">
         <v>0.03</v>
       </c>
@@ -47290,8 +47290,8 @@
       <c r="G214" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H214" s="79"/>
-      <c r="I214" s="79"/>
+      <c r="H214" s="80"/>
+      <c r="I214" s="80"/>
       <c r="J214" s="57">
         <v>0.4</v>
       </c>
@@ -47457,8 +47457,8 @@
       <c r="G215" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H215" s="79"/>
-      <c r="I215" s="79"/>
+      <c r="H215" s="80"/>
+      <c r="I215" s="80"/>
       <c r="J215" s="57">
         <v>3.5</v>
       </c>
@@ -47624,8 +47624,8 @@
       <c r="G216" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H216" s="79"/>
-      <c r="I216" s="79"/>
+      <c r="H216" s="80"/>
+      <c r="I216" s="80"/>
       <c r="J216" s="57">
         <v>2.8</v>
       </c>
@@ -47791,8 +47791,8 @@
       <c r="G217" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H217" s="79"/>
-      <c r="I217" s="79"/>
+      <c r="H217" s="80"/>
+      <c r="I217" s="80"/>
       <c r="J217" s="57">
         <v>0.72</v>
       </c>
@@ -47958,8 +47958,8 @@
       <c r="G218" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H218" s="79"/>
-      <c r="I218" s="79"/>
+      <c r="H218" s="80"/>
+      <c r="I218" s="80"/>
       <c r="J218" s="57">
         <v>0.03</v>
       </c>
@@ -48125,8 +48125,8 @@
       <c r="G219" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H219" s="79"/>
-      <c r="I219" s="79"/>
+      <c r="H219" s="80"/>
+      <c r="I219" s="80"/>
       <c r="J219" s="57">
         <v>0.2</v>
       </c>
@@ -48292,8 +48292,8 @@
       <c r="G220" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H220" s="79"/>
-      <c r="I220" s="79"/>
+      <c r="H220" s="80"/>
+      <c r="I220" s="80"/>
       <c r="J220" s="57">
         <v>0.44</v>
       </c>
@@ -48459,8 +48459,8 @@
       <c r="G221" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H221" s="79"/>
-      <c r="I221" s="79"/>
+      <c r="H221" s="80"/>
+      <c r="I221" s="80"/>
       <c r="J221" s="57">
         <v>7</v>
       </c>
@@ -48626,8 +48626,8 @@
       <c r="G222" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H222" s="79"/>
-      <c r="I222" s="79"/>
+      <c r="H222" s="80"/>
+      <c r="I222" s="80"/>
       <c r="J222" s="57">
         <v>2.34</v>
       </c>
@@ -48793,8 +48793,8 @@
       <c r="G223" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H223" s="79"/>
-      <c r="I223" s="79"/>
+      <c r="H223" s="80"/>
+      <c r="I223" s="80"/>
       <c r="J223" s="57">
         <v>6</v>
       </c>
@@ -48960,8 +48960,8 @@
       <c r="G224" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H224" s="79"/>
-      <c r="I224" s="79"/>
+      <c r="H224" s="80"/>
+      <c r="I224" s="80"/>
       <c r="J224" s="57">
         <v>8</v>
       </c>
@@ -49127,8 +49127,8 @@
       <c r="G225" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H225" s="79"/>
-      <c r="I225" s="79"/>
+      <c r="H225" s="80"/>
+      <c r="I225" s="80"/>
       <c r="J225" s="57">
         <v>0.08</v>
       </c>
@@ -49294,8 +49294,8 @@
       <c r="G226" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H226" s="79"/>
-      <c r="I226" s="79"/>
+      <c r="H226" s="80"/>
+      <c r="I226" s="80"/>
       <c r="J226" s="57">
         <v>1.3</v>
       </c>
@@ -49461,8 +49461,8 @@
       <c r="G227" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H227" s="79"/>
-      <c r="I227" s="79"/>
+      <c r="H227" s="80"/>
+      <c r="I227" s="80"/>
       <c r="J227" s="57">
         <v>2.5</v>
       </c>
@@ -49628,8 +49628,8 @@
       <c r="G228" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H228" s="79"/>
-      <c r="I228" s="79"/>
+      <c r="H228" s="80"/>
+      <c r="I228" s="80"/>
       <c r="J228" s="57">
         <v>42</v>
       </c>
@@ -49795,8 +49795,8 @@
       <c r="G229" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H229" s="79"/>
-      <c r="I229" s="79"/>
+      <c r="H229" s="80"/>
+      <c r="I229" s="80"/>
       <c r="J229" s="57">
         <v>1.1000000000000001</v>
       </c>
@@ -49962,8 +49962,8 @@
       <c r="G230" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H230" s="79"/>
-      <c r="I230" s="79"/>
+      <c r="H230" s="80"/>
+      <c r="I230" s="80"/>
       <c r="J230" s="57">
         <v>1.6</v>
       </c>
@@ -50129,8 +50129,8 @@
       <c r="G231" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H231" s="79"/>
-      <c r="I231" s="79"/>
+      <c r="H231" s="80"/>
+      <c r="I231" s="80"/>
       <c r="J231" s="57">
         <v>60</v>
       </c>
@@ -50296,8 +50296,8 @@
       <c r="G232" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H232" s="79"/>
-      <c r="I232" s="79"/>
+      <c r="H232" s="80"/>
+      <c r="I232" s="80"/>
       <c r="J232" s="57">
         <v>2</v>
       </c>
@@ -50463,8 +50463,8 @@
       <c r="G233" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H233" s="79"/>
-      <c r="I233" s="79"/>
+      <c r="H233" s="80"/>
+      <c r="I233" s="80"/>
       <c r="J233" s="57">
         <v>1</v>
       </c>
@@ -50630,8 +50630,8 @@
       <c r="G234" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H234" s="79"/>
-      <c r="I234" s="79"/>
+      <c r="H234" s="80"/>
+      <c r="I234" s="80"/>
       <c r="J234" s="57">
         <v>0.24</v>
       </c>
@@ -50797,8 +50797,8 @@
       <c r="G235" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H235" s="79"/>
-      <c r="I235" s="79"/>
+      <c r="H235" s="80"/>
+      <c r="I235" s="80"/>
       <c r="J235" s="57">
         <v>1.35</v>
       </c>
@@ -50964,8 +50964,8 @@
       <c r="G236" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H236" s="79"/>
-      <c r="I236" s="79"/>
+      <c r="H236" s="80"/>
+      <c r="I236" s="80"/>
       <c r="J236" s="57">
         <v>0.3</v>
       </c>
@@ -51131,8 +51131,8 @@
       <c r="G237" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H237" s="79"/>
-      <c r="I237" s="79"/>
+      <c r="H237" s="80"/>
+      <c r="I237" s="80"/>
       <c r="J237" s="57">
         <v>1.1200000000000001</v>
       </c>
@@ -51298,8 +51298,8 @@
       <c r="G238" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H238" s="79"/>
-      <c r="I238" s="79"/>
+      <c r="H238" s="80"/>
+      <c r="I238" s="80"/>
       <c r="J238" s="57">
         <v>0.54</v>
       </c>
@@ -51465,8 +51465,8 @@
       <c r="G239" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H239" s="79"/>
-      <c r="I239" s="79"/>
+      <c r="H239" s="80"/>
+      <c r="I239" s="80"/>
       <c r="J239" s="57">
         <v>0.28000000000000003</v>
       </c>
@@ -51632,8 +51632,8 @@
       <c r="G240" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H240" s="79"/>
-      <c r="I240" s="79"/>
+      <c r="H240" s="80"/>
+      <c r="I240" s="80"/>
       <c r="J240" s="57">
         <v>1.3</v>
       </c>
@@ -51799,8 +51799,8 @@
       <c r="G241" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H241" s="79"/>
-      <c r="I241" s="79"/>
+      <c r="H241" s="80"/>
+      <c r="I241" s="80"/>
       <c r="J241" s="57">
         <v>0.06</v>
       </c>
@@ -51966,8 +51966,8 @@
       <c r="G242" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H242" s="79"/>
-      <c r="I242" s="79"/>
+      <c r="H242" s="80"/>
+      <c r="I242" s="80"/>
       <c r="J242" s="57">
         <v>0.06</v>
       </c>
@@ -52133,8 +52133,8 @@
       <c r="G243" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H243" s="79"/>
-      <c r="I243" s="79"/>
+      <c r="H243" s="80"/>
+      <c r="I243" s="80"/>
       <c r="J243" s="57">
         <v>0.52</v>
       </c>
@@ -52300,8 +52300,8 @@
       <c r="G244" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H244" s="79"/>
-      <c r="I244" s="79"/>
+      <c r="H244" s="80"/>
+      <c r="I244" s="80"/>
       <c r="J244" s="57">
         <v>0.05</v>
       </c>
@@ -52467,8 +52467,8 @@
       <c r="G245" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H245" s="79"/>
-      <c r="I245" s="79"/>
+      <c r="H245" s="80"/>
+      <c r="I245" s="80"/>
       <c r="J245" s="57">
         <v>2</v>
       </c>
@@ -52634,8 +52634,8 @@
       <c r="G246" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H246" s="79"/>
-      <c r="I246" s="79"/>
+      <c r="H246" s="80"/>
+      <c r="I246" s="80"/>
       <c r="J246" s="57">
         <v>1</v>
       </c>
@@ -52801,8 +52801,8 @@
       <c r="G247" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H247" s="79"/>
-      <c r="I247" s="79"/>
+      <c r="H247" s="80"/>
+      <c r="I247" s="80"/>
       <c r="J247" s="57">
         <v>0.05</v>
       </c>
@@ -52968,8 +52968,8 @@
       <c r="G248" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H248" s="79"/>
-      <c r="I248" s="79"/>
+      <c r="H248" s="80"/>
+      <c r="I248" s="80"/>
       <c r="J248" s="57">
         <v>0.1</v>
       </c>
@@ -53135,8 +53135,8 @@
       <c r="G249" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H249" s="79"/>
-      <c r="I249" s="79"/>
+      <c r="H249" s="80"/>
+      <c r="I249" s="80"/>
       <c r="J249" s="57">
         <v>0.03</v>
       </c>
@@ -53175,8 +53175,8 @@
       <c r="G250" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H250" s="79"/>
-      <c r="I250" s="79"/>
+      <c r="H250" s="80"/>
+      <c r="I250" s="80"/>
       <c r="J250" s="57">
         <v>0.05</v>
       </c>
@@ -53215,8 +53215,8 @@
       <c r="G251" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H251" s="79"/>
-      <c r="I251" s="79"/>
+      <c r="H251" s="80"/>
+      <c r="I251" s="80"/>
       <c r="J251" s="57">
         <v>0.6</v>
       </c>
@@ -53255,8 +53255,8 @@
       <c r="G252" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H252" s="79"/>
-      <c r="I252" s="79"/>
+      <c r="H252" s="80"/>
+      <c r="I252" s="80"/>
       <c r="J252" s="57">
         <v>0.16</v>
       </c>
@@ -53295,8 +53295,8 @@
       <c r="G253" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H253" s="79"/>
-      <c r="I253" s="79"/>
+      <c r="H253" s="80"/>
+      <c r="I253" s="80"/>
       <c r="J253" s="57">
         <v>1.5</v>
       </c>
@@ -53335,8 +53335,8 @@
       <c r="G254" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H254" s="79"/>
-      <c r="I254" s="79"/>
+      <c r="H254" s="80"/>
+      <c r="I254" s="80"/>
       <c r="J254" s="57">
         <v>1</v>
       </c>
@@ -53375,8 +53375,8 @@
       <c r="G255" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H255" s="79"/>
-      <c r="I255" s="79"/>
+      <c r="H255" s="80"/>
+      <c r="I255" s="80"/>
       <c r="J255" s="57">
         <v>0.04</v>
       </c>
@@ -53415,8 +53415,8 @@
       <c r="G256" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H256" s="79"/>
-      <c r="I256" s="79"/>
+      <c r="H256" s="80"/>
+      <c r="I256" s="80"/>
       <c r="J256" s="57">
         <v>0.09</v>
       </c>
@@ -53455,8 +53455,8 @@
       <c r="G257" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H257" s="79"/>
-      <c r="I257" s="79"/>
+      <c r="H257" s="80"/>
+      <c r="I257" s="80"/>
       <c r="J257" s="57">
         <v>0.12</v>
       </c>
@@ -53495,8 +53495,8 @@
       <c r="G258" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H258" s="79"/>
-      <c r="I258" s="79"/>
+      <c r="H258" s="80"/>
+      <c r="I258" s="80"/>
       <c r="J258" s="57">
         <v>0.04</v>
       </c>
@@ -53535,8 +53535,8 @@
       <c r="G259" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H259" s="79"/>
-      <c r="I259" s="79"/>
+      <c r="H259" s="80"/>
+      <c r="I259" s="80"/>
       <c r="J259" s="57">
         <v>25</v>
       </c>
@@ -53575,8 +53575,8 @@
       <c r="G260" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H260" s="79"/>
-      <c r="I260" s="79"/>
+      <c r="H260" s="80"/>
+      <c r="I260" s="80"/>
       <c r="J260" s="57">
         <v>12</v>
       </c>
@@ -53615,8 +53615,8 @@
       <c r="G261" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H261" s="79"/>
-      <c r="I261" s="79"/>
+      <c r="H261" s="80"/>
+      <c r="I261" s="80"/>
       <c r="J261" s="57">
         <v>5.5</v>
       </c>
@@ -53655,8 +53655,8 @@
       <c r="G262" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H262" s="79"/>
-      <c r="I262" s="79"/>
+      <c r="H262" s="80"/>
+      <c r="I262" s="80"/>
       <c r="J262" s="57">
         <v>0.4</v>
       </c>
@@ -53695,8 +53695,8 @@
       <c r="G263" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H263" s="79"/>
-      <c r="I263" s="79"/>
+      <c r="H263" s="80"/>
+      <c r="I263" s="80"/>
       <c r="J263" s="57">
         <v>0.04</v>
       </c>
@@ -53735,8 +53735,8 @@
       <c r="G264" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H264" s="79"/>
-      <c r="I264" s="79"/>
+      <c r="H264" s="80"/>
+      <c r="I264" s="80"/>
       <c r="J264" s="57">
         <v>28</v>
       </c>
@@ -61747,10 +61747,10 @@
       <c r="G464" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H464" s="79">
+      <c r="H464" s="80">
         <v>1</v>
       </c>
-      <c r="I464" s="79" t="s">
+      <c r="I464" s="80" t="s">
         <v>1518</v>
       </c>
       <c r="J464" s="57">
@@ -61791,8 +61791,8 @@
       <c r="G465" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H465" s="79"/>
-      <c r="I465" s="79"/>
+      <c r="H465" s="80"/>
+      <c r="I465" s="80"/>
       <c r="J465" s="57">
         <v>0.36</v>
       </c>
@@ -61831,8 +61831,8 @@
       <c r="G466" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H466" s="79"/>
-      <c r="I466" s="79"/>
+      <c r="H466" s="80"/>
+      <c r="I466" s="80"/>
       <c r="J466" s="57">
         <v>0.35</v>
       </c>
@@ -61871,8 +61871,8 @@
       <c r="G467" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H467" s="79"/>
-      <c r="I467" s="79"/>
+      <c r="H467" s="80"/>
+      <c r="I467" s="80"/>
       <c r="J467" s="57">
         <v>0.34</v>
       </c>
@@ -61911,8 +61911,8 @@
       <c r="G468" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H468" s="79"/>
-      <c r="I468" s="79"/>
+      <c r="H468" s="80"/>
+      <c r="I468" s="80"/>
       <c r="J468" s="57">
         <v>2.29</v>
       </c>
@@ -61951,8 +61951,8 @@
       <c r="G469" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H469" s="79"/>
-      <c r="I469" s="79"/>
+      <c r="H469" s="80"/>
+      <c r="I469" s="80"/>
       <c r="J469" s="57">
         <v>1.28</v>
       </c>
@@ -61991,8 +61991,8 @@
       <c r="G470" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H470" s="79"/>
-      <c r="I470" s="79"/>
+      <c r="H470" s="80"/>
+      <c r="I470" s="80"/>
       <c r="J470" s="57">
         <v>2.83</v>
       </c>
@@ -62031,8 +62031,8 @@
       <c r="G471" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H471" s="79"/>
-      <c r="I471" s="79"/>
+      <c r="H471" s="80"/>
+      <c r="I471" s="80"/>
       <c r="J471" s="57">
         <v>19.46</v>
       </c>
@@ -62071,8 +62071,8 @@
       <c r="G472" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H472" s="79"/>
-      <c r="I472" s="79"/>
+      <c r="H472" s="80"/>
+      <c r="I472" s="80"/>
       <c r="J472" s="57">
         <v>0.09</v>
       </c>
@@ -62111,8 +62111,8 @@
       <c r="G473" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H473" s="79"/>
-      <c r="I473" s="79"/>
+      <c r="H473" s="80"/>
+      <c r="I473" s="80"/>
       <c r="J473" s="57">
         <v>11.14</v>
       </c>
@@ -62151,8 +62151,8 @@
       <c r="G474" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H474" s="79"/>
-      <c r="I474" s="79"/>
+      <c r="H474" s="80"/>
+      <c r="I474" s="80"/>
       <c r="J474" s="57">
         <v>4.04</v>
       </c>
@@ -62191,8 +62191,8 @@
       <c r="G475" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H475" s="79"/>
-      <c r="I475" s="79"/>
+      <c r="H475" s="80"/>
+      <c r="I475" s="80"/>
       <c r="J475" s="57">
         <v>0.24</v>
       </c>
@@ -62231,8 +62231,8 @@
       <c r="G476" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H476" s="79"/>
-      <c r="I476" s="79"/>
+      <c r="H476" s="80"/>
+      <c r="I476" s="80"/>
       <c r="J476" s="57">
         <v>0.36</v>
       </c>
@@ -62271,8 +62271,8 @@
       <c r="G477" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H477" s="79"/>
-      <c r="I477" s="79"/>
+      <c r="H477" s="80"/>
+      <c r="I477" s="80"/>
       <c r="J477" s="57">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -62311,8 +62311,8 @@
       <c r="G478" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H478" s="79"/>
-      <c r="I478" s="79"/>
+      <c r="H478" s="80"/>
+      <c r="I478" s="80"/>
       <c r="J478" s="57">
         <v>0.11</v>
       </c>
@@ -62351,8 +62351,8 @@
       <c r="G479" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H479" s="79"/>
-      <c r="I479" s="79"/>
+      <c r="H479" s="80"/>
+      <c r="I479" s="80"/>
       <c r="J479" s="57">
         <v>0.14000000000000001</v>
       </c>
@@ -62391,8 +62391,8 @@
       <c r="G480" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H480" s="79"/>
-      <c r="I480" s="79"/>
+      <c r="H480" s="80"/>
+      <c r="I480" s="80"/>
       <c r="J480" s="57">
         <v>0.39</v>
       </c>
@@ -62431,8 +62431,8 @@
       <c r="G481" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H481" s="79"/>
-      <c r="I481" s="79"/>
+      <c r="H481" s="80"/>
+      <c r="I481" s="80"/>
       <c r="J481" s="57">
         <v>0.17</v>
       </c>
@@ -62471,8 +62471,8 @@
       <c r="G482" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H482" s="79"/>
-      <c r="I482" s="79"/>
+      <c r="H482" s="80"/>
+      <c r="I482" s="80"/>
       <c r="J482" s="57">
         <v>0.39</v>
       </c>
@@ -62511,8 +62511,8 @@
       <c r="G483" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H483" s="79"/>
-      <c r="I483" s="79"/>
+      <c r="H483" s="80"/>
+      <c r="I483" s="80"/>
       <c r="J483" s="57">
         <v>0.28999999999999998</v>
       </c>
@@ -62551,8 +62551,8 @@
       <c r="G484" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H484" s="79"/>
-      <c r="I484" s="79"/>
+      <c r="H484" s="80"/>
+      <c r="I484" s="80"/>
       <c r="J484" s="57">
         <v>0.49</v>
       </c>
@@ -62591,8 +62591,8 @@
       <c r="G485" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H485" s="79"/>
-      <c r="I485" s="79"/>
+      <c r="H485" s="80"/>
+      <c r="I485" s="80"/>
       <c r="J485" s="57">
         <v>0.41</v>
       </c>
@@ -62631,8 +62631,8 @@
       <c r="G486" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H486" s="79"/>
-      <c r="I486" s="79"/>
+      <c r="H486" s="80"/>
+      <c r="I486" s="80"/>
       <c r="J486" s="57">
         <v>0.39</v>
       </c>
@@ -62671,8 +62671,8 @@
       <c r="G487" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H487" s="79"/>
-      <c r="I487" s="79"/>
+      <c r="H487" s="80"/>
+      <c r="I487" s="80"/>
       <c r="J487" s="57">
         <v>0.01</v>
       </c>
@@ -62711,8 +62711,8 @@
       <c r="G488" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H488" s="79"/>
-      <c r="I488" s="79"/>
+      <c r="H488" s="80"/>
+      <c r="I488" s="80"/>
       <c r="J488" s="57">
         <v>0.01</v>
       </c>
@@ -62751,8 +62751,8 @@
       <c r="G489" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H489" s="79"/>
-      <c r="I489" s="79"/>
+      <c r="H489" s="80"/>
+      <c r="I489" s="80"/>
       <c r="J489" s="57">
         <v>0.19</v>
       </c>
@@ -62791,8 +62791,8 @@
       <c r="G490" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H490" s="79"/>
-      <c r="I490" s="79"/>
+      <c r="H490" s="80"/>
+      <c r="I490" s="80"/>
       <c r="J490" s="57">
         <v>0.09</v>
       </c>
@@ -62831,8 +62831,8 @@
       <c r="G491" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H491" s="79"/>
-      <c r="I491" s="79"/>
+      <c r="H491" s="80"/>
+      <c r="I491" s="80"/>
       <c r="J491" s="57">
         <v>8.11</v>
       </c>
@@ -62871,8 +62871,8 @@
       <c r="G492" s="56" t="s">
         <v>805</v>
       </c>
-      <c r="H492" s="79"/>
-      <c r="I492" s="79"/>
+      <c r="H492" s="80"/>
+      <c r="I492" s="80"/>
       <c r="J492" s="57">
         <v>0.11</v>
       </c>
@@ -62911,8 +62911,8 @@
       <c r="G493" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H493" s="79"/>
-      <c r="I493" s="79"/>
+      <c r="H493" s="80"/>
+      <c r="I493" s="80"/>
       <c r="J493" s="57">
         <v>0.13</v>
       </c>
@@ -62951,8 +62951,8 @@
       <c r="G494" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H494" s="79"/>
-      <c r="I494" s="79"/>
+      <c r="H494" s="80"/>
+      <c r="I494" s="80"/>
       <c r="J494" s="57">
         <v>0.49</v>
       </c>
@@ -62991,8 +62991,8 @@
       <c r="G495" s="56" t="s">
         <v>817</v>
       </c>
-      <c r="H495" s="79"/>
-      <c r="I495" s="79"/>
+      <c r="H495" s="80"/>
+      <c r="I495" s="80"/>
       <c r="J495" s="57">
         <v>1.82</v>
       </c>
@@ -65293,30 +65293,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H9:H27"/>
-    <mergeCell ref="I9:I27"/>
-    <mergeCell ref="H28:H46"/>
-    <mergeCell ref="I28:I46"/>
-    <mergeCell ref="H47:H62"/>
-    <mergeCell ref="I47:I62"/>
-    <mergeCell ref="H63:H75"/>
-    <mergeCell ref="I63:I75"/>
-    <mergeCell ref="H76:H90"/>
-    <mergeCell ref="I76:I90"/>
-    <mergeCell ref="H91:H110"/>
-    <mergeCell ref="I91:I110"/>
-    <mergeCell ref="H111:H127"/>
-    <mergeCell ref="I111:I127"/>
-    <mergeCell ref="H128:H264"/>
-    <mergeCell ref="I128:I264"/>
-    <mergeCell ref="H265:H291"/>
-    <mergeCell ref="I265:I291"/>
-    <mergeCell ref="H292:H448"/>
-    <mergeCell ref="I292:I448"/>
-    <mergeCell ref="H449:H463"/>
-    <mergeCell ref="I449:I463"/>
     <mergeCell ref="H506:H508"/>
     <mergeCell ref="I506:I508"/>
     <mergeCell ref="H511:H551"/>
@@ -65327,6 +65303,30 @@
     <mergeCell ref="I500:I502"/>
     <mergeCell ref="H503:H505"/>
     <mergeCell ref="I503:I505"/>
+    <mergeCell ref="H265:H291"/>
+    <mergeCell ref="I265:I291"/>
+    <mergeCell ref="H292:H448"/>
+    <mergeCell ref="I292:I448"/>
+    <mergeCell ref="H449:H463"/>
+    <mergeCell ref="I449:I463"/>
+    <mergeCell ref="H91:H110"/>
+    <mergeCell ref="I91:I110"/>
+    <mergeCell ref="H111:H127"/>
+    <mergeCell ref="I111:I127"/>
+    <mergeCell ref="H128:H264"/>
+    <mergeCell ref="I128:I264"/>
+    <mergeCell ref="H47:H62"/>
+    <mergeCell ref="I47:I62"/>
+    <mergeCell ref="H63:H75"/>
+    <mergeCell ref="I63:I75"/>
+    <mergeCell ref="H76:H90"/>
+    <mergeCell ref="I76:I90"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H9:H27"/>
+    <mergeCell ref="I9:I27"/>
+    <mergeCell ref="H28:H46"/>
+    <mergeCell ref="I28:I46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O506" r:id="rId1" xr:uid="{3507F328-EB9F-4719-BF2C-5B53C15E8C9C}"/>

</xml_diff>